<commit_message>
Fix issues with packagejson, erase sample
</commit_message>
<xml_diff>
--- a/Documentation/highLevelTests_Run_1.xlsx
+++ b/Documentation/highLevelTests_Run_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skyward/projects/comp296/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC03CED2-1E0B-8445-9590-079CA94D9129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D75F34-44AE-FD44-9937-431CC24D9F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="1580" windowWidth="22960" windowHeight="21100" xr2:uid="{FD0C20E4-CB01-CA41-8F75-B2A5513064F5}"/>
+    <workbookView xWindow="22920" yWindow="4100" windowWidth="22960" windowHeight="21100" xr2:uid="{FD0C20E4-CB01-CA41-8F75-B2A5513064F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>Test Case</t>
   </si>
@@ -255,13 +255,16 @@
   </si>
   <si>
     <t>Unpinning last routine will not display until after reload. Not fixing.</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,6 +287,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -305,11 +313,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228516EB-DC15-C748-80D4-6F756B42DEAE}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="266" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="266" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,8 +1080,11 @@
       <c r="A51" t="s">
         <v>39</v>
       </c>
-      <c r="B51" t="s">
-        <v>42</v>
+      <c r="B51" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>